<commit_message>
prima implementazione counterfactual che stampa su terminale + uml
</commit_message>
<xml_diff>
--- a/statistiche/performanceMetrics.xlsx
+++ b/statistiche/performanceMetrics.xlsx
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3673469387755102</v>
+        <v>0.3106060606060606</v>
       </c>
       <c r="C2" t="n">
-        <v>0.08035714285714286</v>
+        <v>0.06101190476190476</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1318681318681319</v>
+        <v>0.1019900497512438</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
aggiunta stampa su file excel dei counterfactual
</commit_message>
<xml_diff>
--- a/statistiche/performanceMetrics.xlsx
+++ b/statistiche/performanceMetrics.xlsx
@@ -457,13 +457,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3106060606060606</v>
+        <v>0.352112676056338</v>
       </c>
       <c r="C2" t="n">
-        <v>0.06101190476190476</v>
+        <v>0.0744047619047619</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1019900497512438</v>
+        <v>0.1228501228501228</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
nuovo calcolo di maxPermittedRange, counterfactual sulle trace e con output piu completi e leggibili
</commit_message>
<xml_diff>
--- a/statistiche/performanceMetrics.xlsx
+++ b/statistiche/performanceMetrics.xlsx
@@ -467,19 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7589023310417855</v>
+        <v>0.7613898750257053</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7180442374854482</v>
+        <v>0.7173457508731083</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7369419147848194</v>
+        <v>0.7375309023440424</v>
       </c>
       <c r="E2" t="n">
-        <v>0.4989854475662059</v>
+        <v>0.5034286756980586</v>
       </c>
       <c r="F2" t="n">
-        <v>0.5021814598311271</v>
+        <v>0.5079934600998902</v>
       </c>
     </row>
     <row r="3">

</xml_diff>